<commit_message>
GESTION CAMIONES COMPLETADO GESTION PILOTOS COMPLETADO GESTION USUARIOS COMPLETADO (PODRIA MEJORARSE) CERRAR SESION (COMPLETADO - RESIVISION) LOGIN (COMPLETADO MOMENTANEAMENTE) CREACION DE FICHEROS PARA CADA UNA DE LAS CLASES
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/PINEED.xlsx
+++ b/ProyectoPooDist/excels/PINEED.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Nombre Piloto</t>
   </si>
@@ -41,58 +41,49 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>Sofía</t>
-  </si>
-  <si>
-    <t>Ortega</t>
+    <t>MEME</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>camila.ruiz@gmail.com</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>14/09/2024</t>
+  </si>
+  <si>
+    <t>NEUTRO</t>
+  </si>
+  <si>
+    <t>Andrés</t>
+  </si>
+  <si>
+    <t>Morales</t>
+  </si>
+  <si>
+    <t>andres.morales@gmail.com</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>EN VACACIONES</t>
+  </si>
+  <si>
+    <t>Meme</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>sofia.ortega@gmail.com</t>
-  </si>
-  <si>
-    <t>Masculino</t>
-  </si>
-  <si>
-    <t>14/09/2024</t>
-  </si>
-  <si>
-    <t>EN VACACIONES</t>
-  </si>
-  <si>
-    <t>Camila</t>
-  </si>
-  <si>
-    <t>Ruiz</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>camila.ruiz@gmail.com</t>
-  </si>
-  <si>
-    <t>Femenino</t>
-  </si>
-  <si>
-    <t>NEUTRO</t>
-  </si>
-  <si>
-    <t>Andrés</t>
-  </si>
-  <si>
-    <t>Morales</t>
-  </si>
-  <si>
-    <t>andres.morales@gmail.com</t>
-  </si>
-  <si>
-    <t>Meme</t>
-  </si>
-  <si>
-    <t>Gonzalez</t>
   </si>
   <si>
     <t>a@gmail.com</t>
@@ -140,7 +131,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -183,7 +174,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>3.21321E12</v>
+        <v>2.54645E12</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>11</v>
@@ -192,7 +183,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>1.2352121E7</v>
+        <v>3.2512432E7</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>13</v>
@@ -212,83 +203,54 @@
         <v>17</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>2.54645E12</v>
+        <v>1.32231E12</v>
       </c>
       <c r="D3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="F3" t="n" s="0">
+        <v>1.4215322E7</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>19</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>3.2512432E7</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>20</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="C4" t="n" s="0">
+        <v>3.025564510103E12</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>23</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>1.32231E12</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>18</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>24</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>1.4215322E7</v>
+        <v>1.2124531E7</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>14</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>3.025564510103E12</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>1.2124531E7</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OPTIMIZACION DE DISEÑOS Y PROCESOS NO.13
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/PINEED.xlsx
+++ b/ProyectoPooDist/excels/PINEED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Downloads\PROYECTO CINDY\Proyecto-Poo-Dist\ProyectoPooDist\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517AAE04-8B96-4B9E-B58C-3302BAD7E714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89558E07-16CE-438A-90FE-9D064502FCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>Nombre Piloto</t>
   </si>
@@ -70,45 +70,42 @@
     <t>10/03/2023</t>
   </si>
   <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>carlos.perez@gmail.com</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>23/07/2021</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Fernandez</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>maria.fernandez@pineed.com</t>
+  </si>
+  <si>
+    <t>15/06/2022</t>
+  </si>
+  <si>
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>carlos.perez@gmail.com</t>
-  </si>
-  <si>
-    <t>Masculino</t>
-  </si>
-  <si>
-    <t>23/07/2021</t>
-  </si>
-  <si>
-    <t>INACTIVO</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Fernandez</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>maria.fernandez@pineed.com</t>
-  </si>
-  <si>
-    <t>15/06/2022</t>
-  </si>
-  <si>
     <t>Pedro</t>
   </si>
   <si>
@@ -139,7 +136,7 @@
     <t>Ramirez</t>
   </si>
   <si>
-    <t>jose.ramirez@pineed.com</t>
+    <t>jose.ramirez@gmail.com</t>
   </si>
   <si>
     <t>19/09/2021</t>
@@ -574,13 +571,10 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J12"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -640,7 +634,7 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -648,31 +642,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
       </c>
       <c r="C3">
         <v>2456780000000</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
       <c r="F3">
         <v>12345678</v>
       </c>
       <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -680,19 +674,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>3789010000000</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>87654321</v>
@@ -701,10 +695,10 @@
         <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -712,10 +706,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
       </c>
       <c r="C5">
         <v>1234560000000</v>
@@ -724,19 +718,19 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5">
         <v>65432189</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -744,19 +738,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
       </c>
       <c r="C6">
         <v>1678900000000</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6">
         <v>54321678</v>
@@ -765,10 +759,10 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -776,31 +770,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
       </c>
       <c r="C7">
         <v>2123450000000</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7">
         <v>43219876</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -808,10 +802,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
         <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
       </c>
       <c r="C8">
         <v>3567890000000</v>
@@ -820,7 +814,7 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8">
         <v>32165498</v>
@@ -829,10 +823,10 @@
         <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -840,31 +834,31 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
         <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
       </c>
       <c r="C9">
         <v>4987650000000</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9">
         <v>21987654</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -872,10 +866,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
       </c>
       <c r="C10">
         <v>4654320000000</v>
@@ -884,19 +878,19 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10">
         <v>87654321</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
@@ -904,19 +898,19 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>5432100000000</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11">
         <v>76543210</v>
@@ -925,10 +919,10 @@
         <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -936,10 +930,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
         <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
       </c>
       <c r="C12">
         <v>7890120000000</v>
@@ -948,7 +942,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12">
         <v>54321098</v>
@@ -957,10 +951,10 @@
         <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>

</xml_diff>